<commit_message>
updated lab2 stock solution
</commit_message>
<xml_diff>
--- a/topic02/book-b/archives/stockPrices_lab2_solution.xlsx
+++ b/topic02/book-b/archives/stockPrices_lab2_solution.xlsx
@@ -263,2022 +263,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Functions on Arrays - template '!$E$3</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Duke Energy Stock </c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-2.3399444634638063E-2"/>
-                  <c:y val="-0.26082412112279069"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'Functions on Arrays - template '!$D$4:$D$178</c:f>
-              <c:numCache>
-                <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="175"/>
-                <c:pt idx="0">
-                  <c:v>-2.8632061512498972E-3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>-1.5194720363435775E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.8878978754786419E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2.0812198017934665E-2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>6.1816510284721333E-3</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6.9082404225633224E-3</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>4.2213382157548759E-2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>-3.6231396526946812E-2</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2.328951485450324E-2</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2.7663279564206007E-2</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>4.3629977912082465E-2</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>2.9315544388002535E-2</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>-3.179826168331884E-2</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>4.8277757876973679E-2</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>-1.5112952997701294E-2</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>2.0550174751576469E-2</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>1.7924162116924588E-2</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>3.535536713008354E-2</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>1.0999881888155871E-2</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>4.9197760692578335E-2</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>7.0434471114575181E-3</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>2.8426587376603443E-3</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>-1.9987836058499683E-2</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>2.394705705020073E-2</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>1.9570602004381984E-2</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>1.2518948972710817E-2</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>3.8792661243837456E-2</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>-6.4699250170469236E-2</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>-7.5257447960486246E-3</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>3.0851535762571346E-2</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>3.9787331386417914E-2</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>4.2659999011137491E-2</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>8.4965534941463527E-3</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>-5.0714834366809821E-3</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>0.10230659165059017</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>-7.4467127542783104E-2</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>-5.8467491619120418E-2</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>-2.1708367435427242E-2</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>-1.8426233301897538E-2</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>-1.3592893899637262E-2</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>2.809691636712916E-2</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>-1.0478506829378123E-3</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>3.1456595040144836E-2</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>2.239298525651701E-2</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>6.3256517221926059E-2</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>-2.2929094870601432E-3</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>3.6193000710687595E-2</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>8.3928475095282604E-2</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>-4.8611803170382606E-2</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>6.6515783274589638E-2</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>-5.5388380132376618E-2</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>-8.5531653633770133E-2</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>1.4651468311863144E-2</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>5.7132760645483123E-2</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>2.8114744036660498E-2</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>-3.7675141059320766E-2</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>1.7614546700982087E-2</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>5.5779015582807137E-2</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>-1.9959865222177731E-2</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>3.5100104155946166E-2</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>3.3009321348136535E-2</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>7.1521977088891908E-2</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>1.9581606407012827E-4</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>5.1720558420882315E-2</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>8.9772214920969498E-2</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>8.1952736214643773E-2</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>-0.11645654382051443</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>-8.9549885511070959E-2</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>7.7911357772817548E-3</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>-7.7798346417088868E-2</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>-0.18563648644598751</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>-9.5180786774375359E-2</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>1.2116797460712942E-2</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>-9.9083004864562122E-3</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>-8.98835504310454E-2</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>1.0617586652650165E-2</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>4.6450939660056381E-2</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>-5.9774122413739049E-3</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>-3.5379707842082095E-2</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>-6.3113909602276946E-2</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>-8.6659298048018304E-3</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>-4.5042789369416157E-2</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>1.4713557788708606E-2</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>3.5168283637491062E-2</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>1.2781559065278813E-2</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>-3.2504500841186675E-2</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>-1.7976930819991094E-2</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>3.2030723748061214E-2</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>4.2379836237605301E-2</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>9.9304839152859412E-3</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>-2.2088305664389823E-2</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>1.3961172524527271E-2</c:v>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v>1.2536835916847028E-2</c:v>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v>1.6332505122359679E-2</c:v>
-                </c:pt>
-                <c:pt idx="94">
-                  <c:v>3.1021836917226073E-2</c:v>
-                </c:pt>
-                <c:pt idx="95">
-                  <c:v>2.4269376195304011E-2</c:v>
-                </c:pt>
-                <c:pt idx="96">
-                  <c:v>2.105112458799209E-2</c:v>
-                </c:pt>
-                <c:pt idx="97">
-                  <c:v>5.072924191958309E-3</c:v>
-                </c:pt>
-                <c:pt idx="98">
-                  <c:v>8.6604285391806066E-5</c:v>
-                </c:pt>
-                <c:pt idx="99">
-                  <c:v>-3.1404913585891703E-2</c:v>
-                </c:pt>
-                <c:pt idx="100">
-                  <c:v>1.2082373675144375E-2</c:v>
-                </c:pt>
-                <c:pt idx="101">
-                  <c:v>1.1034733969458945E-2</c:v>
-                </c:pt>
-                <c:pt idx="102">
-                  <c:v>4.529940641520396E-4</c:v>
-                </c:pt>
-                <c:pt idx="103">
-                  <c:v>2.5147961230518261E-2</c:v>
-                </c:pt>
-                <c:pt idx="104">
-                  <c:v>-9.528500142413687E-4</c:v>
-                </c:pt>
-                <c:pt idx="105">
-                  <c:v>3.4581237676988605E-2</c:v>
-                </c:pt>
-                <c:pt idx="106">
-                  <c:v>-1.7899994313773929E-2</c:v>
-                </c:pt>
-                <c:pt idx="107">
-                  <c:v>6.9249074268589216E-3</c:v>
-                </c:pt>
-                <c:pt idx="108">
-                  <c:v>-1.1285467972359155E-2</c:v>
-                </c:pt>
-                <c:pt idx="109">
-                  <c:v>3.5336451864729147E-2</c:v>
-                </c:pt>
-                <c:pt idx="110">
-                  <c:v>-1.4268747689802155E-4</c:v>
-                </c:pt>
-                <c:pt idx="111">
-                  <c:v>2.9512223385105795E-2</c:v>
-                </c:pt>
-                <c:pt idx="112">
-                  <c:v>-2.031351934767037E-2</c:v>
-                </c:pt>
-                <c:pt idx="113">
-                  <c:v>-1.930275225452871E-2</c:v>
-                </c:pt>
-                <c:pt idx="114">
-                  <c:v>1.8726934874337724E-2</c:v>
-                </c:pt>
-                <c:pt idx="115">
-                  <c:v>-2.5615747968515911E-2</c:v>
-                </c:pt>
-                <c:pt idx="116">
-                  <c:v>3.1942491193192112E-2</c:v>
-                </c:pt>
-                <c:pt idx="117">
-                  <c:v>3.7868779461133012E-2</c:v>
-                </c:pt>
-                <c:pt idx="118">
-                  <c:v>1.391695587821374E-2</c:v>
-                </c:pt>
-                <c:pt idx="119">
-                  <c:v>9.3203368022064838E-3</c:v>
-                </c:pt>
-                <c:pt idx="120">
-                  <c:v>2.284720571713859E-3</c:v>
-                </c:pt>
-                <c:pt idx="121">
-                  <c:v>-3.4892238215330364E-2</c:v>
-                </c:pt>
-                <c:pt idx="122">
-                  <c:v>1.7829189249312503E-2</c:v>
-                </c:pt>
-                <c:pt idx="123">
-                  <c:v>1.2011024205564368E-2</c:v>
-                </c:pt>
-                <c:pt idx="124">
-                  <c:v>-1.6933393494544095E-2</c:v>
-                </c:pt>
-                <c:pt idx="125">
-                  <c:v>-1.6494220669989047E-2</c:v>
-                </c:pt>
-                <c:pt idx="126">
-                  <c:v>1.2135100829125884E-2</c:v>
-                </c:pt>
-                <c:pt idx="127">
-                  <c:v>1.7128882262967212E-2</c:v>
-                </c:pt>
-                <c:pt idx="128">
-                  <c:v>4.9518899306471208E-2</c:v>
-                </c:pt>
-                <c:pt idx="129">
-                  <c:v>7.1032253560451564E-3</c:v>
-                </c:pt>
-                <c:pt idx="130">
-                  <c:v>5.3504268464946513E-2</c:v>
-                </c:pt>
-                <c:pt idx="131">
-                  <c:v>-1.2016232567985653E-2</c:v>
-                </c:pt>
-                <c:pt idx="132">
-                  <c:v>1.7715343790636197E-2</c:v>
-                </c:pt>
-                <c:pt idx="133">
-                  <c:v>1.6093506478773681E-2</c:v>
-                </c:pt>
-                <c:pt idx="134">
-                  <c:v>1.125862601085219E-2</c:v>
-                </c:pt>
-                <c:pt idx="135">
-                  <c:v>4.9645665489287727E-2</c:v>
-                </c:pt>
-                <c:pt idx="136">
-                  <c:v>7.7927350029476733E-2</c:v>
-                </c:pt>
-                <c:pt idx="137">
-                  <c:v>8.3228742528296627E-3</c:v>
-                </c:pt>
-                <c:pt idx="138">
-                  <c:v>-1.7149844258839787E-2</c:v>
-                </c:pt>
-                <c:pt idx="139">
-                  <c:v>-2.7797493671422965E-2</c:v>
-                </c:pt>
-                <c:pt idx="140">
-                  <c:v>-6.2229277129875436E-2</c:v>
-                </c:pt>
-                <c:pt idx="141">
-                  <c:v>5.550058467611222E-2</c:v>
-                </c:pt>
-                <c:pt idx="142">
-                  <c:v>8.2914421028757151E-2</c:v>
-                </c:pt>
-                <c:pt idx="143">
-                  <c:v>-0.11656116844786664</c:v>
-                </c:pt>
-                <c:pt idx="144">
-                  <c:v>4.8695443903156652E-3</c:v>
-                </c:pt>
-                <c:pt idx="145">
-                  <c:v>-8.2299871837899052E-2</c:v>
-                </c:pt>
-                <c:pt idx="146">
-                  <c:v>-7.5214343275906148E-2</c:v>
-                </c:pt>
-                <c:pt idx="147">
-                  <c:v>-9.122942297125956E-3</c:v>
-                </c:pt>
-                <c:pt idx="148">
-                  <c:v>-6.3384682784413518E-2</c:v>
-                </c:pt>
-                <c:pt idx="149">
-                  <c:v>3.6080076252758407E-2</c:v>
-                </c:pt>
-                <c:pt idx="150">
-                  <c:v>-2.0984886675167722E-2</c:v>
-                </c:pt>
-                <c:pt idx="151">
-                  <c:v>-1.5696373666933345E-2</c:v>
-                </c:pt>
-                <c:pt idx="152">
-                  <c:v>7.545292033896033E-3</c:v>
-                </c:pt>
-                <c:pt idx="153">
-                  <c:v>7.2484350433373146E-2</c:v>
-                </c:pt>
-                <c:pt idx="154">
-                  <c:v>1.7937188329115412E-2</c:v>
-                </c:pt>
-                <c:pt idx="155">
-                  <c:v>-8.5256615246989922E-2</c:v>
-                </c:pt>
-                <c:pt idx="156">
-                  <c:v>-6.6255605887467039E-2</c:v>
-                </c:pt>
-                <c:pt idx="157">
-                  <c:v>-1.0798221205900169E-2</c:v>
-                </c:pt>
-                <c:pt idx="158">
-                  <c:v>-2.5354152249423972E-2</c:v>
-                </c:pt>
-                <c:pt idx="159">
-                  <c:v>5.0772876986084174E-3</c:v>
-                </c:pt>
-                <c:pt idx="160">
-                  <c:v>7.4007010555980454E-2</c:v>
-                </c:pt>
-                <c:pt idx="161">
-                  <c:v>-6.635854393013127E-2</c:v>
-                </c:pt>
-                <c:pt idx="162">
-                  <c:v>-9.6831090416541171E-2</c:v>
-                </c:pt>
-                <c:pt idx="163">
-                  <c:v>3.4050246450141819E-2</c:v>
-                </c:pt>
-                <c:pt idx="164">
-                  <c:v>4.0451932227232121E-3</c:v>
-                </c:pt>
-                <c:pt idx="165">
-                  <c:v>-8.3456133710587313E-2</c:v>
-                </c:pt>
-                <c:pt idx="166">
-                  <c:v>-4.9617849736629414E-3</c:v>
-                </c:pt>
-                <c:pt idx="167">
-                  <c:v>-5.4966292284748544E-2</c:v>
-                </c:pt>
-                <c:pt idx="168">
-                  <c:v>5.8928157588211842E-2</c:v>
-                </c:pt>
-                <c:pt idx="169">
-                  <c:v>-1.647625326436223E-2</c:v>
-                </c:pt>
-                <c:pt idx="170">
-                  <c:v>2.3651631156730649E-2</c:v>
-                </c:pt>
-                <c:pt idx="171">
-                  <c:v>-2.2158698229963615E-2</c:v>
-                </c:pt>
-                <c:pt idx="172">
-                  <c:v>-3.1279977258077872E-2</c:v>
-                </c:pt>
-                <c:pt idx="173">
-                  <c:v>9.2323812122223556E-2</c:v>
-                </c:pt>
-                <c:pt idx="174">
-                  <c:v>-2.0313062610448358E-2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'Functions on Arrays - template '!$E$4:$E$178</c:f>
-              <c:numCache>
-                <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="175"/>
-                <c:pt idx="0">
-                  <c:v>1.1167138864952873E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>-2.8159323685853343E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4.2823366914983882E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>-3.5925388660600951E-2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4.4828153602362211E-2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>4.8378011258130875E-3</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.4655434718172784E-2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2.3134267446924487E-2</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>-1.3681713970213486E-2</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>-1.4073500327499622E-2</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>7.1506988955139961E-2</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1.7799064738143931E-2</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>-6.804724493894454E-2</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>5.0557729808596699E-2</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>8.5503824458129235E-3</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>-0.1058287900751869</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>3.5307033284416159E-2</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>4.7067510857985946E-2</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>1.8470588211003378E-2</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>7.4645873276560762E-2</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>-3.3472803659802025E-4</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>-1.6595136903010281E-2</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>1.3921338518608014E-2</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>1.6690311313052921E-4</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>-3.396831626376863E-2</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>-2.0441465517900576E-2</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>4.7921114144363106E-2</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>3.6994337646125544E-2</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>1.9637437017252114E-2</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>4.3971577312865145E-3</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>-6.8511466928531037E-3</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>-3.1874521981083849E-2</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>5.3822305623651645E-2</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>3.2927030994847672E-2</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>2.1309217524017397E-2</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>5.5548259528042869E-2</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>3.0621879590610628E-2</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>-1.2280137946591087E-2</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>4.2809157213146206E-3</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>1.7933078749567344E-2</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>2.719678534882717E-2</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>8.8011730507392954E-3</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>1.9815563990466429E-2</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>3.9665102687966381E-3</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>1.4679978926943869E-2</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>-2.3692019258980498E-2</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>2.7958333128729911E-2</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>3.0384976012385923E-2</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>1.8495201208999348E-2</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>6.6683226432004528E-2</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>2.5290858194812632E-3</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>-3.6060104934585294E-2</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>2.7989443220917565E-2</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>-2.0075289050894142E-3</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>3.7674287936445405E-3</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>-4.0439435193726232E-2</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>3.1421338004873393E-2</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>6.7835721506927668E-2</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>4.8154186148665701E-3</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>1.6220955823538708E-2</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>1.5934403077824351E-2</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>5.9327346776551944E-2</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>3.0734927046334157E-2</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>4.08219945202552E-2</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>-3.6266177984394493E-2</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>6.119556102691992E-2</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>-0.10234626863839412</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>9.3924964045466273E-3</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>-3.6199116679428996E-2</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>-3.6580932003612704E-2</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>-6.2187940560226189E-2</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>-5.1519836276086358E-4</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>4.905134399258544E-3</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>1.1452493731787729E-2</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>-6.1425040539709035E-2</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>2.0896282726412412E-2</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>2.5459623611320349E-2</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>1.7690367681850491E-2</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>-4.9664672314364521E-2</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>-7.8273680561424253E-2</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>1.8883880881723769E-2</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>4.3286392113121623E-2</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>2.5387127487359631E-2</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>1.8830072903874388E-2</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>8.6054405614066132E-2</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>-7.2086253004408143E-2</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>-6.5531125503539928E-2</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>-3.8526118759078569E-2</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>1.1094177284399598E-2</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>3.0608486601449148E-2</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>9.8377576498766481E-3</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>1.997070864794968E-2</c:v>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v>4.5919854773772271E-2</c:v>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v>1.275256389739134E-2</c:v>
-                </c:pt>
-                <c:pt idx="94">
-                  <c:v>4.6520015634892699E-2</c:v>
-                </c:pt>
-                <c:pt idx="95">
-                  <c:v>6.7453881395316551E-3</c:v>
-                </c:pt>
-                <c:pt idx="96">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="97">
-                  <c:v>3.1803281977703365E-2</c:v>
-                </c:pt>
-                <c:pt idx="98">
-                  <c:v>3.9791472803256879E-2</c:v>
-                </c:pt>
-                <c:pt idx="99">
-                  <c:v>-2.0390511553359813E-2</c:v>
-                </c:pt>
-                <c:pt idx="100">
-                  <c:v>-1.1865916550972979E-3</c:v>
-                </c:pt>
-                <c:pt idx="101">
-                  <c:v>2.6131536464436732E-2</c:v>
-                </c:pt>
-                <c:pt idx="102">
-                  <c:v>1.2863883361909828E-2</c:v>
-                </c:pt>
-                <c:pt idx="103">
-                  <c:v>3.2265915696656836E-2</c:v>
-                </c:pt>
-                <c:pt idx="104">
-                  <c:v>2.1561575440105413E-2</c:v>
-                </c:pt>
-                <c:pt idx="105">
-                  <c:v>2.6369359118967459E-2</c:v>
-                </c:pt>
-                <c:pt idx="106">
-                  <c:v>-9.7009106249007812E-2</c:v>
-                </c:pt>
-                <c:pt idx="107">
-                  <c:v>6.3859119248064243E-3</c:v>
-                </c:pt>
-                <c:pt idx="108">
-                  <c:v>-1.8737326666971039E-2</c:v>
-                </c:pt>
-                <c:pt idx="109">
-                  <c:v>-6.5652279978147899E-3</c:v>
-                </c:pt>
-                <c:pt idx="110">
-                  <c:v>7.8556602481022877E-2</c:v>
-                </c:pt>
-                <c:pt idx="111">
-                  <c:v>-5.0198744492355542E-2</c:v>
-                </c:pt>
-                <c:pt idx="112">
-                  <c:v>4.1230074509595011E-2</c:v>
-                </c:pt>
-                <c:pt idx="113">
-                  <c:v>3.7029238637613565E-2</c:v>
-                </c:pt>
-                <c:pt idx="114">
-                  <c:v>1.7693668068925011E-2</c:v>
-                </c:pt>
-                <c:pt idx="115">
-                  <c:v>5.5752709618058151E-2</c:v>
-                </c:pt>
-                <c:pt idx="116">
-                  <c:v>2.1390382487494423E-3</c:v>
-                </c:pt>
-                <c:pt idx="117">
-                  <c:v>4.0792254301067567E-2</c:v>
-                </c:pt>
-                <c:pt idx="118">
-                  <c:v>6.9258440470055166E-2</c:v>
-                </c:pt>
-                <c:pt idx="119">
-                  <c:v>3.3214879946440665E-2</c:v>
-                </c:pt>
-                <c:pt idx="120">
-                  <c:v>4.2058343328060507E-2</c:v>
-                </c:pt>
-                <c:pt idx="121">
-                  <c:v>5.7916736466718362E-2</c:v>
-                </c:pt>
-                <c:pt idx="122">
-                  <c:v>1.7447641869802771E-2</c:v>
-                </c:pt>
-                <c:pt idx="123">
-                  <c:v>-4.0840521444508213E-2</c:v>
-                </c:pt>
-                <c:pt idx="124">
-                  <c:v>-7.0385113665716079E-2</c:v>
-                </c:pt>
-                <c:pt idx="125">
-                  <c:v>2.8585384744651884E-2</c:v>
-                </c:pt>
-                <c:pt idx="126">
-                  <c:v>2.3296998426884177E-2</c:v>
-                </c:pt>
-                <c:pt idx="127">
-                  <c:v>6.0733750424607914E-2</c:v>
-                </c:pt>
-                <c:pt idx="128">
-                  <c:v>0.12534868892355222</c:v>
-                </c:pt>
-                <c:pt idx="129">
-                  <c:v>9.5087879690271358E-3</c:v>
-                </c:pt>
-                <c:pt idx="130">
-                  <c:v>1.8752223749183609E-2</c:v>
-                </c:pt>
-                <c:pt idx="131">
-                  <c:v>4.1971925312916894E-2</c:v>
-                </c:pt>
-                <c:pt idx="132">
-                  <c:v>-1.1217167530924924E-2</c:v>
-                </c:pt>
-                <c:pt idx="133">
-                  <c:v>-0.12856929696932234</c:v>
-                </c:pt>
-                <c:pt idx="134">
-                  <c:v>2.9362646885874172E-2</c:v>
-                </c:pt>
-                <c:pt idx="135">
-                  <c:v>0.11324788049099219</c:v>
-                </c:pt>
-                <c:pt idx="136">
-                  <c:v>0.19004360288786507</c:v>
-                </c:pt>
-                <c:pt idx="137">
-                  <c:v>7.3792332191082333E-2</c:v>
-                </c:pt>
-                <c:pt idx="138">
-                  <c:v>-0.21337582528997409</c:v>
-                </c:pt>
-                <c:pt idx="139">
-                  <c:v>-0.13761287949711348</c:v>
-                </c:pt>
-                <c:pt idx="140">
-                  <c:v>-1.031468660183168E-2</c:v>
-                </c:pt>
-                <c:pt idx="141">
-                  <c:v>-2.2324620705233986E-2</c:v>
-                </c:pt>
-                <c:pt idx="142">
-                  <c:v>4.6735077107459035E-2</c:v>
-                </c:pt>
-                <c:pt idx="143">
-                  <c:v>-0.31644425721140351</c:v>
-                </c:pt>
-                <c:pt idx="144">
-                  <c:v>6.1630875045882522E-2</c:v>
-                </c:pt>
-                <c:pt idx="145">
-                  <c:v>-0.19889093970871699</c:v>
-                </c:pt>
-                <c:pt idx="146">
-                  <c:v>-2.896845090048732E-2</c:v>
-                </c:pt>
-                <c:pt idx="147">
-                  <c:v>-0.17270374689875331</c:v>
-                </c:pt>
-                <c:pt idx="148">
-                  <c:v>1.4020848241938451E-2</c:v>
-                </c:pt>
-                <c:pt idx="149">
-                  <c:v>6.8459079475225809E-2</c:v>
-                </c:pt>
-                <c:pt idx="150">
-                  <c:v>2.0063556680680661E-2</c:v>
-                </c:pt>
-                <c:pt idx="151">
-                  <c:v>-0.11852215882122645</c:v>
-                </c:pt>
-                <c:pt idx="152">
-                  <c:v>8.2575915327587068E-2</c:v>
-                </c:pt>
-                <c:pt idx="153">
-                  <c:v>-5.3683199637458053E-2</c:v>
-                </c:pt>
-                <c:pt idx="154">
-                  <c:v>1.4484932921367013E-2</c:v>
-                </c:pt>
-                <c:pt idx="155">
-                  <c:v>-3.7719543795455966E-2</c:v>
-                </c:pt>
-                <c:pt idx="156">
-                  <c:v>2.5172327743367279E-2</c:v>
-                </c:pt>
-                <c:pt idx="157">
-                  <c:v>-1.0199950595819745E-2</c:v>
-                </c:pt>
-                <c:pt idx="158">
-                  <c:v>-0.15868548040541647</c:v>
-                </c:pt>
-                <c:pt idx="159">
-                  <c:v>-1.6249196890796999E-2</c:v>
-                </c:pt>
-                <c:pt idx="160">
-                  <c:v>8.9799258853585764E-2</c:v>
-                </c:pt>
-                <c:pt idx="161">
-                  <c:v>4.7720207809686985E-2</c:v>
-                </c:pt>
-                <c:pt idx="162">
-                  <c:v>0.11494690276563554</c:v>
-                </c:pt>
-                <c:pt idx="163">
-                  <c:v>-0.15330350932589581</c:v>
-                </c:pt>
-                <c:pt idx="164">
-                  <c:v>-5.3464847901058446E-2</c:v>
-                </c:pt>
-                <c:pt idx="165">
-                  <c:v>4.6118393074371829E-2</c:v>
-                </c:pt>
-                <c:pt idx="166">
-                  <c:v>7.8551018366358472E-3</c:v>
-                </c:pt>
-                <c:pt idx="167">
-                  <c:v>0.13662517295894011</c:v>
-                </c:pt>
-                <c:pt idx="168">
-                  <c:v>0.20086513450612362</c:v>
-                </c:pt>
-                <c:pt idx="169">
-                  <c:v>9.0225091592725695E-2</c:v>
-                </c:pt>
-                <c:pt idx="170">
-                  <c:v>-3.3003762907998543E-2</c:v>
-                </c:pt>
-                <c:pt idx="171">
-                  <c:v>2.2524334578486294E-2</c:v>
-                </c:pt>
-                <c:pt idx="172">
-                  <c:v>9.0879853767550062E-2</c:v>
-                </c:pt>
-                <c:pt idx="173">
-                  <c:v>7.9162193396342784E-2</c:v>
-                </c:pt>
-                <c:pt idx="174">
-                  <c:v>-0.16423370556814595</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-31E4-46C1-BF23-9BF7E9B7D7EB}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="714457984"/>
-        <c:axId val="714454656"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="714457984"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="714454656"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="714454656"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="714457984"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>762000</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>685800</xdr:colOff>
-      <xdr:row>52</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2605,8 +589,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N179"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D18" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView tabSelected="1" topLeftCell="D28" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3224,10 +1208,7 @@
       <c r="G21" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H21" s="21">
-        <f>SLOPE(E4:E178,D4:D178)</f>
-        <v>0.48627082066856381</v>
-      </c>
+      <c r="H21" s="21"/>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
@@ -3283,10 +1264,7 @@
       <c r="G23" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="H23" s="22">
-        <f>INTERCEPT(E4:E178,D4:D178)</f>
-        <v>5.0536105766135339E-3</v>
-      </c>
+      <c r="H23" s="22"/>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
@@ -3342,10 +1320,7 @@
       <c r="G25" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H25" s="21">
-        <f>CORREL(E4:E178,D4:D178)</f>
-        <v>0.33353572873695747</v>
-      </c>
+      <c r="H25" s="21"/>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
@@ -3401,10 +1376,7 @@
       <c r="G27" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H27" s="22">
-        <f>RSQ(E4:E178,D4:D178)</f>
-        <v>0.11124608234409328</v>
-      </c>
+      <c r="H27" s="22"/>
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
@@ -6337,7 +4309,6 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
-  <drawing r:id="rId2"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>